<commit_message>
Alteracao exercicio módulo 08
</commit_message>
<xml_diff>
--- a/Resumo/Modulo 04 -Tecnicas de testes/Tabelas de decisao.xlsx
+++ b/Resumo/Modulo 04 -Tecnicas de testes/Tabelas de decisao.xlsx
@@ -1,14 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="510" yWindow="555" windowWidth="15015" windowHeight="5580" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Validacao de senha" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Validacao voto" sheetId="3" r:id="rId6"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Validacao de senha" sheetId="2" r:id="rId2"/>
+    <sheet name="Validacao voto" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhCaHGzPCT+MOXKjP4IS/HvtKn45A=="/>
@@ -95,27 +98,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="4">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -125,7 +129,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -135,98 +139,95 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="double">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -416,25 +417,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B4:F998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="14.14"/>
-    <col customWidth="1" min="3" max="19" width="8.71"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="19" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4">
+    <row r="4" spans="2:6">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,41 +454,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:6">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:6">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F6" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -494,24 +497,24 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8">
+    <row r="8" spans="2:6">
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E8" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F8" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:6">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1498,29 +1501,27 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B4:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="21.29"/>
-    <col customWidth="1" min="3" max="22" width="8.71"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="22" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4">
+    <row r="4" spans="2:16">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1549,123 +1550,195 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:16">
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3">
-        <v>1.0</v>
+        <v>0</v>
       </c>
       <c r="F5" s="3">
-        <v>1.0</v>
+        <v>0</v>
       </c>
       <c r="G5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10">
+        <v>1</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0</v>
+      </c>
+      <c r="O5" s="10">
+        <v>1</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:16">
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F6" s="3">
-        <v>1.0</v>
+        <v>0</v>
       </c>
       <c r="G6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
+        <v>1</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0</v>
+      </c>
+      <c r="M6" s="10">
+        <v>1</v>
+      </c>
+      <c r="N6" s="10">
+        <v>1</v>
+      </c>
+      <c r="O6" s="10">
+        <v>1</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:16">
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <v>1</v>
+      </c>
+      <c r="K7" s="10">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0</v>
+      </c>
+      <c r="N7" s="10">
+        <v>1</v>
+      </c>
+      <c r="O7" s="10">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <v>1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:16">
       <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <v>1</v>
+      </c>
+      <c r="L8" s="10">
+        <v>1</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0</v>
+      </c>
+      <c r="O8" s="10">
+        <v>1</v>
+      </c>
+      <c r="P8" s="10">
+        <v>0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:16">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1678,36 +1751,36 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10">
+    <row r="10" spans="2:16">
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E10" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F10" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G10" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I10" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J10" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="2:16">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2695,29 +2768,25 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B4:J1002"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="22.14"/>
-    <col customWidth="1" min="3" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4">
+    <row r="4" spans="2:10">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2746,123 +2815,123 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:10">
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E5" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F5" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I5" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J5" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:10">
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D6" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E6" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G6" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H6" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I6" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J6" s="11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:10">
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H7" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I7" s="11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:10">
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G8" s="11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J8" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:10">
       <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
@@ -2875,62 +2944,62 @@
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10">
+    <row r="10" spans="2:10">
       <c r="B10" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E10" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F10" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G10" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H10" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I10" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J10" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="2:10">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D11" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E11" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G11" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H11" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I11" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J11" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -3916,9 +3985,7 @@
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>